<commit_message>
Vergleiche in Excel erzeugt
</commit_message>
<xml_diff>
--- a/07_Test/VerlgeicheJARTAvsArta.Standard/ContinousUniform/ContinousUniform.xlsx
+++ b/07_Test/VerlgeicheJARTAvsArta.Standard/ContinousUniform/ContinousUniform.xlsx
@@ -220,34 +220,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.82263007158858004</c:v>
+                  <c:v>-0.81498163899999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83693485582818095</c:v>
+                  <c:v>0.82957343100000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.76253590460485599</c:v>
+                  <c:v>-0.75336583599999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74131028747684902</c:v>
+                  <c:v>0.72498680800000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.69807963369263504</c:v>
+                  <c:v>-0.67801120500000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67068065495217799</c:v>
+                  <c:v>0.64629482800000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.635117809130894</c:v>
+                  <c:v>-0.61080151800000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.60915703708783697</c:v>
+                  <c:v>0.58487081500000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.58037950442274699</c:v>
+                  <c:v>-0.55086908499999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55814627838435604</c:v>
+                  <c:v>0.52466367700000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -295,34 +295,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.41658215937611098</c:v>
+                  <c:v>-0.39831064700000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50900789708610905</c:v>
+                  <c:v>0.49813321199999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.29926337981151202</c:v>
+                  <c:v>-0.28012198199999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27696673425437401</c:v>
+                  <c:v>0.26849856500000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.198788138363303</c:v>
+                  <c:v>-0.17589776100000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16508882450613299</c:v>
+                  <c:v>0.14984826900000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.12587437032688301</c:v>
+                  <c:v>-9.6415809000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.81088720137758E-2</c:v>
+                  <c:v>8.1421004000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-8.9957758334422003E-2</c:v>
+                  <c:v>-5.6172544999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.5134542911019606E-2</c:v>
+                  <c:v>3.4392677000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -640,34 +640,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.82263007200000005</c:v>
+                  <c:v>-0.81498163899999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.160214621</c:v>
+                  <c:v>0.165378358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9270642999999998E-2</c:v>
+                  <c:v>5.9118495E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9553697E-2</c:v>
+                  <c:v>2.2692252999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8860399999999996E-3</c:v>
+                  <c:v>7.1027249999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5897899999999999E-3</c:v>
+                  <c:v>5.5048579999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3362299999999999E-3</c:v>
+                  <c:v>9.0313800000000005E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5045240000000002E-3</c:v>
+                  <c:v>5.5202760000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1518850000000001E-3</c:v>
+                  <c:v>6.9461729999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.586952E-3</c:v>
+                  <c:v>3.1189389999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -715,34 +715,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.41658215900000001</c:v>
+                  <c:v>-0.39831064700000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33546720200000002</c:v>
+                  <c:v>0.33948183999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9191147999999999E-2</c:v>
+                  <c:v>6.0479102999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0124430000000001E-3</c:v>
+                  <c:v>1.3505471999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.1560657E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1.478902E-3</c:v>
+                  <c:v>1.585202E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>-5.8799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0.00E+00">
-                  <c:v>6.3199999999999997E-4</c:v>
+                  <c:v>1.0784597E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.6346099999999999E-3</c:v>
+                  <c:v>4.7563659999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.5718683000000001E-2</c:v>
+                  <c:v>-2.0034599999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.6765030000000003E-3</c:v>
+                  <c:v>-1.3077780000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1057,145 +1057,145 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>-0.13607666936149401</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>0.60243102129747395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>-0.97804858159049701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>0.99808702196337895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>-0.99288834884616195</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>0.57607430958199801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>-0.97102481691891995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>0.54437506168370697</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>-0.98717143250827</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.53902383600000003</c:v>
+                  <c:v>0.72271398151315103</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>-0.98484397472014795</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>0.99669984057556904</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>-0.74951303392744395</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.53902383600000003</c:v>
+                  <c:v>0.98506063842470104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.30466079400000001</c:v>
+                  <c:v>-0.85694675925589103</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>0.95960119067726501</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>-0.96914612855070104</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>0.99442415798450301</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.53902383600000003</c:v>
+                  <c:v>-0.998222503474679</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.30466079400000001</c:v>
+                  <c:v>0.79397092130176605</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.82983947700000005</c:v>
+                  <c:v>-0.64081577798731104</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>0.32477883835170501</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>-0.94706640303688605</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>0.99398263801590803</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.53902383600000003</c:v>
+                  <c:v>-0.94232257069444203</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.30466079400000001</c:v>
+                  <c:v>0.99637027867547101</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.82983947700000005</c:v>
+                  <c:v>-0.83542222109859599</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.743675062</c:v>
+                  <c:v>0.99997569325921398</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>-0.97444869680603896</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>0.98645368657840304</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>-0.230302416770816</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.53902383600000003</c:v>
+                  <c:v>-0.222801571325631</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.30466079400000001</c:v>
+                  <c:v>0.56907043817608705</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.82983947700000005</c:v>
+                  <c:v>-9.0034963797028994E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.743675062</c:v>
+                  <c:v>-0.98894882855571598</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.64884471099999996</c:v>
+                  <c:v>0.97310487070405505</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>-0.99374245072564005</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>0.99400641304801496</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.206222712</c:v>
+                  <c:v>-0.75228541797162496</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.53902383600000003</c:v>
+                  <c:v>0.69019237208681405</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.30466079400000001</c:v>
+                  <c:v>-0.99951307340295903</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.82983947700000005</c:v>
+                  <c:v>0.98909376477512101</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.743675062</c:v>
+                  <c:v>-0.99797526313780405</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-0.64884471099999996</c:v>
+                  <c:v>0.968036182323044</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.715142481</c:v>
+                  <c:v>-0.997127100892645</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.76382998899999999</c:v>
+                  <c:v>0.99996712125568199</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.72917588499999997</c:v>
+                  <c:v>-0.99999429615323698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5222,8 +5222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A704BB88-10B1-4106-BB98-8DB4641D6F90}">
   <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5312,7 +5312,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0.76382998899999999</v>
+        <v>-0.13607666936149401</v>
       </c>
       <c r="I12">
         <v>-0.346867212124437</v>
@@ -5326,19 +5326,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>-0.82263007158858004</v>
+        <v>-0.81498163899999998</v>
       </c>
       <c r="B13">
-        <v>-0.41658215937611098</v>
+        <v>-0.39831064700000002</v>
       </c>
       <c r="D13">
-        <v>-0.82263007200000005</v>
+        <v>-0.81498163899999998</v>
       </c>
       <c r="E13">
-        <v>-0.41658215900000001</v>
+        <v>-0.39831064700000002</v>
       </c>
       <c r="H13">
-        <v>0.76382998899999999</v>
+        <v>0.60243102129747395</v>
       </c>
       <c r="I13">
         <v>0.120173005411793</v>
@@ -5352,19 +5352,19 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0.83693485582818095</v>
+        <v>0.82957343100000003</v>
       </c>
       <c r="B14">
-        <v>0.50900789708610905</v>
+        <v>0.49813321199999999</v>
       </c>
       <c r="D14">
-        <v>0.160214621</v>
+        <v>0.165378358</v>
       </c>
       <c r="E14">
-        <v>0.33546720200000002</v>
+        <v>0.33948183999999998</v>
       </c>
       <c r="H14">
-        <v>-0.72917588499999997</v>
+        <v>-0.97804858159049701</v>
       </c>
       <c r="I14">
         <v>0.54199316609078196</v>
@@ -5378,19 +5378,19 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>-0.76253590460485599</v>
+        <v>-0.75336583599999996</v>
       </c>
       <c r="B15">
-        <v>-0.29926337981151202</v>
+        <v>-0.28012198199999999</v>
       </c>
       <c r="D15">
-        <v>5.9270642999999998E-2</v>
+        <v>5.9118495E-2</v>
       </c>
       <c r="E15">
-        <v>5.9191147999999999E-2</v>
+        <v>6.0479102999999999E-2</v>
       </c>
       <c r="H15">
-        <v>0.76382998899999999</v>
+        <v>0.99808702196337895</v>
       </c>
       <c r="I15">
         <v>-0.48404818424096202</v>
@@ -5404,19 +5404,19 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>0.74131028747684902</v>
+        <v>0.72498680800000004</v>
       </c>
       <c r="B16">
-        <v>0.27696673425437401</v>
+        <v>0.26849856500000002</v>
       </c>
       <c r="D16">
-        <v>2.9553697E-2</v>
+        <v>2.2692252999999999E-2</v>
       </c>
       <c r="E16">
-        <v>7.0124430000000001E-3</v>
+        <v>1.3505471999999999E-2</v>
       </c>
       <c r="H16">
-        <v>-0.72917588499999997</v>
+        <v>-0.99288834884616195</v>
       </c>
       <c r="I16">
         <v>0.43978135885004999</v>
@@ -5430,19 +5430,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>-0.69807963369263504</v>
+        <v>-0.67801120500000001</v>
       </c>
       <c r="B17">
-        <v>-0.198788138363303</v>
+        <v>-0.17589776100000001</v>
       </c>
       <c r="D17">
-        <v>8.8860399999999996E-3</v>
+        <v>7.1027249999999998E-3</v>
       </c>
       <c r="E17">
-        <v>-1.1560657E-2</v>
+        <v>1.585202E-3</v>
       </c>
       <c r="H17">
-        <v>-0.206222712</v>
+        <v>0.57607430958199801</v>
       </c>
       <c r="I17">
         <v>-0.59096705310572994</v>
@@ -5456,19 +5456,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>0.67068065495217799</v>
+        <v>0.64629482800000004</v>
       </c>
       <c r="B18">
-        <v>0.16508882450613299</v>
+        <v>0.14984826900000001</v>
       </c>
       <c r="D18">
-        <v>5.5897899999999999E-3</v>
-      </c>
-      <c r="E18">
-        <v>-1.478902E-3</v>
+        <v>5.5048579999999996E-3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>-5.8799999999999998E-4</v>
       </c>
       <c r="H18">
-        <v>0.76382998899999999</v>
+        <v>-0.97102481691891995</v>
       </c>
       <c r="I18">
         <v>0.68373873430885201</v>
@@ -5482,19 +5482,19 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>-0.635117809130894</v>
+        <v>-0.61080151800000004</v>
       </c>
       <c r="B19">
-        <v>-0.12587437032688301</v>
+        <v>-9.6415809000000005E-2</v>
       </c>
       <c r="D19">
-        <v>4.3362299999999999E-3</v>
+        <v>9.0313800000000005E-4</v>
       </c>
       <c r="E19" s="1">
-        <v>6.3199999999999997E-4</v>
+        <v>1.0784597E-2</v>
       </c>
       <c r="H19">
-        <v>-0.72917588499999997</v>
+        <v>0.54437506168370697</v>
       </c>
       <c r="I19">
         <v>0.13830543752862601</v>
@@ -5508,19 +5508,19 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>0.60915703708783697</v>
+        <v>0.58487081500000004</v>
       </c>
       <c r="B20">
-        <v>9.81088720137758E-2</v>
+        <v>8.1421004000000005E-2</v>
       </c>
       <c r="D20">
-        <v>4.5045240000000002E-3</v>
+        <v>5.5202760000000002E-3</v>
       </c>
       <c r="E20">
-        <v>-2.6346099999999999E-3</v>
+        <v>4.7563659999999997E-3</v>
       </c>
       <c r="H20">
-        <v>-0.206222712</v>
+        <v>-0.98717143250827</v>
       </c>
       <c r="I20">
         <v>-0.643634981492056</v>
@@ -5534,19 +5534,19 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>-0.58037950442274699</v>
+        <v>-0.55086908499999998</v>
       </c>
       <c r="B21">
-        <v>-8.9957758334422003E-2</v>
+        <v>-5.6172544999999997E-2</v>
       </c>
       <c r="D21">
-        <v>1.1518850000000001E-3</v>
+        <v>6.9461729999999999E-3</v>
       </c>
       <c r="E21">
-        <v>-1.5718683000000001E-2</v>
+        <v>-2.0034599999999999E-3</v>
       </c>
       <c r="H21">
-        <v>-0.53902383600000003</v>
+        <v>0.72271398151315103</v>
       </c>
       <c r="I21">
         <v>-0.10418704768440799</v>
@@ -5560,19 +5560,19 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>0.55814627838435604</v>
+        <v>0.52466367700000005</v>
       </c>
       <c r="B22">
-        <v>7.5134542911019606E-2</v>
+        <v>3.4392677000000003E-2</v>
       </c>
       <c r="D22">
-        <v>3.586952E-3</v>
+        <v>3.1189389999999998E-3</v>
       </c>
       <c r="E22">
-        <v>4.6765030000000003E-3</v>
+        <v>-1.3077780000000001E-2</v>
       </c>
       <c r="H22">
-        <v>0.76382998899999999</v>
+        <v>-0.98484397472014795</v>
       </c>
       <c r="I22">
         <v>0.54939220735604399</v>
@@ -5586,7 +5586,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H23">
-        <v>-0.72917588499999997</v>
+        <v>0.99669984057556904</v>
       </c>
       <c r="I23">
         <v>-0.65231271359315501</v>
@@ -5600,7 +5600,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H24">
-        <v>-0.206222712</v>
+        <v>-0.74951303392744395</v>
       </c>
       <c r="I24">
         <v>0.76597670039769705</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H25">
-        <v>-0.53902383600000003</v>
+        <v>0.98506063842470104</v>
       </c>
       <c r="I25">
         <v>-0.12589935539626501</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H26">
-        <v>0.30466079400000001</v>
+        <v>-0.85694675925589103</v>
       </c>
       <c r="I26">
         <v>0.185463289681117</v>
@@ -5642,7 +5642,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H27">
-        <v>0.76382998899999999</v>
+        <v>0.95960119067726501</v>
       </c>
       <c r="I27">
         <v>0.59459436492623097</v>
@@ -5656,7 +5656,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H28">
-        <v>-0.72917588499999997</v>
+        <v>-0.96914612855070104</v>
       </c>
       <c r="I28">
         <v>0.30145337526246402</v>
@@ -5670,7 +5670,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H29">
-        <v>-0.206222712</v>
+        <v>0.99442415798450301</v>
       </c>
       <c r="I29">
         <v>0.69043431705245695</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H30">
-        <v>-0.53902383600000003</v>
+        <v>-0.998222503474679</v>
       </c>
       <c r="I30">
         <v>-1.9223027519778E-3</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H31">
-        <v>0.30466079400000001</v>
+        <v>0.79397092130176605</v>
       </c>
       <c r="I31">
         <v>0.88376844322018999</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H32">
-        <v>-0.82983947700000005</v>
+        <v>-0.64081577798731104</v>
       </c>
       <c r="I32">
         <v>0.21689519362478499</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="33" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H33">
-        <v>0.76382998899999999</v>
+        <v>0.32477883835170501</v>
       </c>
       <c r="I33">
         <v>-0.74736346641373597</v>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="34" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H34">
-        <v>-0.72917588499999997</v>
+        <v>-0.94706640303688605</v>
       </c>
       <c r="I34">
         <v>0.37222685221905399</v>
@@ -5754,7 +5754,7 @@
     </row>
     <row r="35" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H35">
-        <v>-0.206222712</v>
+        <v>0.99398263801590803</v>
       </c>
       <c r="I35">
         <v>0.38823228234903201</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="36" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H36">
-        <v>-0.53902383600000003</v>
+        <v>-0.94232257069444203</v>
       </c>
       <c r="I36">
         <v>0.402143038922536</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="37" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H37">
-        <v>0.30466079400000001</v>
+        <v>0.99637027867547101</v>
       </c>
       <c r="I37">
         <v>0.272829168627376</v>
@@ -5796,7 +5796,7 @@
     </row>
     <row r="38" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H38">
-        <v>-0.82983947700000005</v>
+        <v>-0.83542222109859599</v>
       </c>
       <c r="I38">
         <v>0.43894193891562899</v>
@@ -5810,7 +5810,7 @@
     </row>
     <row r="39" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H39">
-        <v>0.743675062</v>
+        <v>0.99997569325921398</v>
       </c>
       <c r="I39" s="1">
         <v>-3.78091649708811E-4</v>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="40" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H40">
-        <v>0.76382998899999999</v>
+        <v>-0.97444869680603896</v>
       </c>
       <c r="I40">
         <v>0.76515123296205101</v>
@@ -5838,7 +5838,7 @@
     </row>
     <row r="41" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H41">
-        <v>-0.72917588499999997</v>
+        <v>0.98645368657840304</v>
       </c>
       <c r="I41">
         <v>-0.41448621419117498</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="42" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H42">
-        <v>-0.206222712</v>
+        <v>-0.230302416770816</v>
       </c>
       <c r="I42">
         <v>0.659318543552606</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="43" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H43">
-        <v>-0.53902383600000003</v>
+        <v>-0.222801571325631</v>
       </c>
       <c r="I43">
         <v>-0.36086851550029603</v>
@@ -5880,7 +5880,7 @@
     </row>
     <row r="44" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H44">
-        <v>0.30466079400000001</v>
+        <v>0.56907043817608705</v>
       </c>
       <c r="I44">
         <v>0.53035369774129204</v>
@@ -5894,7 +5894,7 @@
     </row>
     <row r="45" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H45">
-        <v>-0.82983947700000005</v>
+        <v>-9.0034963797028994E-2</v>
       </c>
       <c r="I45">
         <v>-9.1654589343101001E-2</v>
@@ -5908,7 +5908,7 @@
     </row>
     <row r="46" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H46">
-        <v>0.743675062</v>
+        <v>-0.98894882855571598</v>
       </c>
       <c r="I46">
         <v>2.3411295679998299E-2</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="47" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H47">
-        <v>-0.64884471099999996</v>
+        <v>0.97310487070405505</v>
       </c>
       <c r="I47">
         <v>9.4377890917122606E-2</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="48" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H48">
-        <v>0.76382998899999999</v>
+        <v>-0.99374245072564005</v>
       </c>
       <c r="I48">
         <v>0.17792165078191399</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="49" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H49">
-        <v>-0.72917588499999997</v>
+        <v>0.99400641304801496</v>
       </c>
       <c r="I49">
         <v>0.36849598088380697</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="50" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H50">
-        <v>-0.206222712</v>
+        <v>-0.75228541797162496</v>
       </c>
       <c r="I50">
         <v>-0.45639896249985801</v>
@@ -5978,7 +5978,7 @@
     </row>
     <row r="51" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H51">
-        <v>-0.53902383600000003</v>
+        <v>0.69019237208681405</v>
       </c>
       <c r="I51">
         <v>0.56225049772832003</v>
@@ -5992,7 +5992,7 @@
     </row>
     <row r="52" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H52">
-        <v>0.30466079400000001</v>
+        <v>-0.99951307340295903</v>
       </c>
       <c r="I52">
         <v>0.88454361166039497</v>
@@ -6006,7 +6006,7 @@
     </row>
     <row r="53" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H53">
-        <v>-0.82983947700000005</v>
+        <v>0.98909376477512101</v>
       </c>
       <c r="I53">
         <v>-0.35131844755584501</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="54" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H54">
-        <v>0.743675062</v>
+        <v>-0.99797526313780405</v>
       </c>
       <c r="I54">
         <v>-0.562777342797256</v>
@@ -6034,7 +6034,7 @@
     </row>
     <row r="55" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H55">
-        <v>-0.64884471099999996</v>
+        <v>0.968036182323044</v>
       </c>
       <c r="I55">
         <v>0.181383710646631</v>
@@ -6048,7 +6048,7 @@
     </row>
     <row r="56" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H56">
-        <v>0.715142481</v>
+        <v>-0.997127100892645</v>
       </c>
       <c r="I56">
         <v>-0.35897657274026301</v>
@@ -6062,7 +6062,7 @@
     </row>
     <row r="57" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H57">
-        <v>0.76382998899999999</v>
+        <v>0.99996712125568199</v>
       </c>
       <c r="I57">
         <v>-0.14659318290014201</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="58" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H58">
-        <v>-0.72917588499999997</v>
+        <v>-0.99999429615323698</v>
       </c>
       <c r="I58">
         <v>0.311342808269301</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="59" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H59">
-        <v>-0.206222712</v>
+        <v>0.99999710843679601</v>
       </c>
       <c r="I59">
         <v>-0.71699723996741904</v>
@@ -6104,7 +6104,7 @@
     </row>
     <row r="60" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H60">
-        <v>-0.53902383600000003</v>
+        <v>-0.999899249973636</v>
       </c>
       <c r="I60">
         <v>-0.215727282972518</v>
@@ -6118,7 +6118,7 @@
     </row>
     <row r="61" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H61">
-        <v>0.30466079400000001</v>
+        <v>0.99997925649900798</v>
       </c>
       <c r="I61">
         <v>-0.75935152552660401</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="62" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H62">
-        <v>-0.82983947700000005</v>
+        <v>-0.99999827043295697</v>
       </c>
       <c r="I62">
         <v>-0.23880761267959699</v>
@@ -6146,7 +6146,7 @@
     </row>
     <row r="63" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H63">
-        <v>0.743675062</v>
+        <v>0.99925518809305802</v>
       </c>
       <c r="I63">
         <v>-0.78229554468810603</v>
@@ -6160,7 +6160,7 @@
     </row>
     <row r="64" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H64">
-        <v>-0.64884471099999996</v>
+        <v>-0.99881887892918197</v>
       </c>
       <c r="I64">
         <v>0.62584768625357101</v>
@@ -6174,7 +6174,7 @@
     </row>
     <row r="65" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H65">
-        <v>0.715142481</v>
+        <v>0.999688649466697</v>
       </c>
       <c r="I65">
         <v>-0.39565306795114502</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="66" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H66">
-        <v>-0.91829931600000003</v>
+        <v>-0.99964582127545198</v>
       </c>
       <c r="I66">
         <v>0.96374986037766897</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="67" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H67">
-        <v>0.76382998899999999</v>
+        <v>0.98809610382206703</v>
       </c>
       <c r="I67">
         <v>-0.96631464538816203</v>
@@ -6216,7 +6216,7 @@
     </row>
     <row r="68" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H68">
-        <v>-0.72917588499999997</v>
+        <v>-0.991312498472668</v>
       </c>
       <c r="I68">
         <v>0.59483879207165602</v>
@@ -6230,7 +6230,7 @@
     </row>
     <row r="69" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H69">
-        <v>-0.206222712</v>
+        <v>0.99987511090645098</v>
       </c>
       <c r="I69">
         <v>-0.451801243594049</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="70" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H70">
-        <v>-0.53902383600000003</v>
+        <v>-0.93080685876303804</v>
       </c>
       <c r="I70">
         <v>-0.30946306962409798</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="71" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H71">
-        <v>0.30466079400000001</v>
+        <v>0.99646264862549305</v>
       </c>
       <c r="I71">
         <v>-0.24816429337040299</v>
@@ -6272,7 +6272,7 @@
     </row>
     <row r="72" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H72">
-        <v>-0.82983947700000005</v>
+        <v>-0.99953703976071095</v>
       </c>
       <c r="I72">
         <v>0.757211065052938</v>
@@ -6286,7 +6286,7 @@
     </row>
     <row r="73" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H73">
-        <v>0.743675062</v>
+        <v>0.99914748950550403</v>
       </c>
       <c r="I73">
         <v>-0.21990221865548301</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="74" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H74">
-        <v>-0.64884471099999996</v>
+        <v>-0.99596529538263001</v>
       </c>
       <c r="I74">
         <v>-0.14665902969678099</v>
@@ -6314,7 +6314,7 @@
     </row>
     <row r="75" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H75">
-        <v>0.715142481</v>
+        <v>0.99942074675135695</v>
       </c>
       <c r="I75">
         <v>-0.61998540220938203</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="76" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H76">
-        <v>-0.91829931600000003</v>
+        <v>-0.99999212403822302</v>
       </c>
       <c r="I76">
         <v>-0.189442456083738</v>
@@ -6342,7 +6342,7 @@
     </row>
     <row r="77" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H77">
-        <v>0.99455469399999996</v>
+        <v>0.99999999995290301</v>
       </c>
       <c r="I77">
         <v>-0.41145491584510802</v>
@@ -6356,7 +6356,7 @@
     </row>
     <row r="78" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H78">
-        <v>0.76382998899999999</v>
+        <v>-0.98083819484039103</v>
       </c>
       <c r="I78">
         <v>0.41721905487591399</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="79" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H79">
-        <v>-0.72917588499999997</v>
+        <v>0.99999988306389298</v>
       </c>
       <c r="I79">
         <v>-0.60273260177281796</v>
@@ -6384,7 +6384,7 @@
     </row>
     <row r="80" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H80">
-        <v>-0.206222712</v>
+        <v>-0.99988715290116004</v>
       </c>
       <c r="I80">
         <v>0.84816568141172499</v>
@@ -6398,7 +6398,7 @@
     </row>
     <row r="81" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H81">
-        <v>-0.53902383600000003</v>
+        <v>0.99999999188090005</v>
       </c>
       <c r="I81">
         <v>-0.98276529556020198</v>
@@ -6412,7 +6412,7 @@
     </row>
     <row r="82" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H82">
-        <v>0.30466079400000001</v>
+        <v>-0.99997303529442005</v>
       </c>
       <c r="I82">
         <v>0.66629363707191502</v>
@@ -6426,7 +6426,7 @@
     </row>
     <row r="83" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H83">
-        <v>-0.82983947700000005</v>
+        <v>0.999943034503744</v>
       </c>
       <c r="I83">
         <v>-0.59437568818100595</v>
@@ -6440,7 +6440,7 @@
     </row>
     <row r="84" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H84">
-        <v>0.743675062</v>
+        <v>-0.99998628946099499</v>
       </c>
       <c r="I84">
         <v>0.78998236033772196</v>
@@ -6454,7 +6454,7 @@
     </row>
     <row r="85" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H85">
-        <v>-0.64884471099999996</v>
+        <v>0.992186840581187</v>
       </c>
       <c r="I85">
         <v>0.48739584555392901</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="86" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H86">
-        <v>0.715142481</v>
+        <v>-0.99960595851622103</v>
       </c>
       <c r="I86">
         <v>0.87591042217600601</v>
@@ -6482,7 +6482,7 @@
     </row>
     <row r="87" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H87">
-        <v>-0.91829931600000003</v>
+        <v>0.99992031909423695</v>
       </c>
       <c r="I87">
         <v>0.96078872607188004</v>
@@ -6496,7 +6496,7 @@
     </row>
     <row r="88" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H88">
-        <v>0.99455469399999996</v>
+        <v>-0.99981209247709701</v>
       </c>
       <c r="I88">
         <v>0.755682277017792</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="89" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H89">
-        <v>-0.99538997900000004</v>
+        <v>0.98604835355532205</v>
       </c>
       <c r="I89">
         <v>0.82559983601801701</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="90" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H90">
-        <v>0.76382998899999999</v>
+        <v>-0.999984830022704</v>
       </c>
       <c r="I90">
         <v>-0.45718198587846198</v>
@@ -6538,7 +6538,7 @@
     </row>
     <row r="91" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H91">
-        <v>-0.72917588499999997</v>
+        <v>0.80138583432924904</v>
       </c>
       <c r="I91">
         <v>0.28323136730752702</v>
@@ -6552,7 +6552,7 @@
     </row>
     <row r="92" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H92">
-        <v>-0.206222712</v>
+        <v>-0.91713259289362703</v>
       </c>
       <c r="I92">
         <v>-0.39632946671639702</v>
@@ -6566,7 +6566,7 @@
     </row>
     <row r="93" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H93">
-        <v>-0.53902383600000003</v>
+        <v>0.86085857013102896</v>
       </c>
       <c r="I93">
         <v>-0.64268256588752404</v>
@@ -6580,7 +6580,7 @@
     </row>
     <row r="94" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H94">
-        <v>0.30466079400000001</v>
+        <v>-0.92680024291102603</v>
       </c>
       <c r="I94">
         <v>-0.60588172714364996</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="95" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H95">
-        <v>-0.82983947700000005</v>
+        <v>0.36163340330082699</v>
       </c>
       <c r="I95">
         <v>-0.327928180999426</v>
@@ -6608,7 +6608,7 @@
     </row>
     <row r="96" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H96">
-        <v>0.743675062</v>
+        <v>-0.99864532682993201</v>
       </c>
       <c r="I96">
         <v>-0.618217825982177</v>
@@ -6622,7 +6622,7 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H97">
-        <v>-0.64884471099999996</v>
+        <v>0.55760281791984001</v>
       </c>
       <c r="I97">
         <v>0.38137660667273399</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H98">
-        <v>0.715142481</v>
+        <v>-0.99225520927645505</v>
       </c>
       <c r="I98">
         <v>-5.1674850444839097E-2</v>
@@ -6650,7 +6650,7 @@
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H99">
-        <v>-0.91829931600000003</v>
+        <v>0.95223119096075703</v>
       </c>
       <c r="I99">
         <v>0.40806244189128199</v>
@@ -6664,7 +6664,7 @@
     </row>
     <row r="100" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H100">
-        <v>0.99455469399999996</v>
+        <v>-0.91829941476340504</v>
       </c>
       <c r="I100">
         <v>-0.62727397715355204</v>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="101" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H101">
-        <v>-0.99538997900000004</v>
+        <v>0.99748333410550105</v>
       </c>
       <c r="I101">
         <v>0.77290253232148098</v>
@@ -6692,7 +6692,7 @@
     </row>
     <row r="102" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H102">
-        <v>0.97180241199999995</v>
+        <v>-0.99997250877333899</v>
       </c>
       <c r="I102">
         <v>-0.75454550678086996</v>
@@ -6706,7 +6706,7 @@
     </row>
     <row r="103" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H103">
-        <v>0.76382998899999999</v>
+        <v>0.96822117750817904</v>
       </c>
       <c r="I103">
         <v>0.75085488278958401</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="104" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H104">
-        <v>-0.72917588499999997</v>
+        <v>-0.91238025004041401</v>
       </c>
       <c r="I104">
         <v>-0.92066590525148995</v>
@@ -6734,7 +6734,7 @@
     </row>
     <row r="105" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H105">
-        <v>-0.206222712</v>
+        <v>0.94440095221415299</v>
       </c>
       <c r="I105">
         <v>0.85198271163601602</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="106" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H106">
-        <v>-0.53902383600000003</v>
+        <v>-0.91583125545855404</v>
       </c>
       <c r="I106">
         <v>0.24417518861312701</v>
@@ -6762,7 +6762,7 @@
     </row>
     <row r="107" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H107">
-        <v>0.30466079400000001</v>
+        <v>0.96361901617696399</v>
       </c>
       <c r="I107">
         <v>-0.226209447638092</v>
@@ -6776,7 +6776,7 @@
     </row>
     <row r="108" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H108">
-        <v>-0.82983947700000005</v>
+        <v>-0.90141030361281105</v>
       </c>
       <c r="I108">
         <v>0.68937720927912804</v>
@@ -6790,7 +6790,7 @@
     </row>
     <row r="109" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H109">
-        <v>0.743675062</v>
+        <v>0.96285048838131404</v>
       </c>
       <c r="I109">
         <v>0.76561790777602601</v>
@@ -6804,7 +6804,7 @@
     </row>
     <row r="110" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H110">
-        <v>-0.64884471099999996</v>
+        <v>-0.92406283894860297</v>
       </c>
       <c r="I110">
         <v>0.21482865138731699</v>
@@ -6818,7 +6818,7 @@
     </row>
     <row r="111" spans="8:13" x14ac:dyDescent="0.3">
       <c r="H111">
-        <v>0.715142481</v>
+        <v>0.89443888949419803</v>
       </c>
       <c r="I111">
         <v>-0.26810441452685901</v>

</xml_diff>